<commit_message>
[CODE] Updated TFE ScarDoc to include missing classes
</commit_message>
<xml_diff>
--- a/TFE/Data/scar/ScarDoc_TFE.xlsx
+++ b/TFE/Data/scar/ScarDoc_TFE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Dawn of War Soulstorm\TFE\Data\scar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46686BF-BB97-4524-BD9F-F581EEDB103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055AE751-8119-4EDD-912F-AF000C4695A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="65">
   <si>
     <t>Class Name</t>
   </si>
@@ -208,6 +208,18 @@
   </si>
   <si>
     <t>This is either self limiting or zombie, defined by programmer. Will default to self limiting which will destroy after 1 tick. Must explicitly be set to zombie</t>
+  </si>
+  <si>
+    <t>AutoBaseBuildingManager</t>
+  </si>
+  <si>
+    <t>SquadDataHistory</t>
+  </si>
+  <si>
+    <t>SquadData, FixedLengthTable</t>
+  </si>
+  <si>
+    <t>CriticalScars\AutoBaseBuilder\Classes</t>
   </si>
 </sst>
 </file>
@@ -575,7 +587,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -830,13 +842,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>51</v>
@@ -851,7 +863,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>41</v>
@@ -872,7 +884,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>41</v>
@@ -892,92 +904,92 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E16" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F16" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="B17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="D17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B18" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="6" t="s">
+      <c r="F18" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="4"/>
+      <c r="G18" s="6"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>41</v>
@@ -998,7 +1010,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>41</v>
@@ -1018,29 +1030,29 @@
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="3"/>
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>41</v>
@@ -1061,7 +1073,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>41</v>
@@ -1082,7 +1094,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>41</v>
@@ -1103,7 +1115,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>41</v>
@@ -1123,77 +1135,77 @@
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D27" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="4"/>
+      <c r="G27" s="6"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="4"/>
+      <c r="A28" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" s="6"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>51</v>
@@ -1208,13 +1220,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>51</v>
@@ -1229,13 +1241,13 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>51</v>
@@ -1250,45 +1262,87 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="4"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+      <c r="D33" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="6"/>
+      <c r="G35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>